<commit_message>
Xong So sánh theo tháng của Đối tác - Loại hình
</commit_message>
<xml_diff>
--- a/DongAERP/Content/Report/ReportDetailtByPartnerLHForOne.xlsx
+++ b/DongAERP/Content/Report/ReportDetailtByPartnerLHForOne.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DongAERP\DongAERP\Content\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE7C6A3-E90D-46F7-917C-110229937FF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8075CBF8-4936-40EA-A4C1-F6A5B68F4262}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FDADBC8A-6B6C-45FD-98E5-87326587A42E}"/>
   </bookViews>
@@ -33,13 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Từ:</t>
-  </si>
-  <si>
-    <t>Đến:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Đơn vị:</t>
   </si>
@@ -63,6 +57,9 @@
   </si>
   <si>
     <t>Quy USD</t>
+  </si>
+  <si>
+    <t>1. Theo doanh số đối tác - loại hình dịch vụ</t>
   </si>
 </sst>
 </file>
@@ -135,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -160,6 +157,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -478,13 +478,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3B6D35-F82E-4989-A479-5B01F28891A5}">
   <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:F35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" customWidth="1"/>
     <col min="3" max="3" width="30.5546875" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
     <col min="5" max="5" width="22.21875" customWidth="1"/>
@@ -502,7 +502,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -543,13 +543,9 @@
       <c r="R2" s="10"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="D4" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M6" s="5"/>
@@ -562,6 +558,10 @@
       <c r="T6" s="5"/>
     </row>
     <row r="7" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="14"/>
       <c r="M7" s="7"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
@@ -627,33 +627,34 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E34" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="E35" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>7</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>